<commit_message>
Fix match database with Kirkeby and Ward, 2022 Reference dates
</commit_message>
<xml_diff>
--- a/outputs/matrices.xlsx
+++ b/outputs/matrices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R-local-git\parametra\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0F6E29-8B56-4BB7-B720-6CB6B892208C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1390A6C6-8945-4986-A152-7C2A7E3FCE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="270" windowWidth="29010" windowHeight="15210" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="param" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="107">
   <si>
     <t>Basic reproduction number</t>
   </si>
@@ -171,9 +171,6 @@
   </si>
   <si>
     <t>Percentage of parameters available for each pathogen</t>
-  </si>
-  <si>
-    <t>Pathogen</t>
   </si>
   <si>
     <t>NA</t>
@@ -2447,7 +2444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D22E2B9B-73A2-43E9-BAF1-CF037AA0748E}">
   <dimension ref="B1:W22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
@@ -2459,67 +2456,67 @@
   <sheetData>
     <row r="1" spans="2:23" ht="161.25" x14ac:dyDescent="0.25">
       <c r="C1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
@@ -3612,7 +3609,7 @@
     </row>
     <row r="18" spans="2:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" s="7">
         <v>14</v>
@@ -5636,7 +5633,7 @@
     </row>
     <row r="20" spans="2:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="7">
         <v>2</v>
@@ -6026,8 +6023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5934845F-E484-4B29-B836-AC4766B1459E}">
   <dimension ref="B2:AR15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AG3" sqref="AG3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6037,134 +6034,131 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:44" ht="267.75" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
       <c r="C2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AN2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="AN2" s="2" t="s">
+      <c r="AO2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AP2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="AQ2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="AR2" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="3" spans="2:44" ht="15.75" x14ac:dyDescent="0.25">
@@ -7479,7 +7473,7 @@
     </row>
     <row r="13" spans="2:44" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
Update matrices.xlsx after changing "study" to "Study" in "Diagnostic test" table
</commit_message>
<xml_diff>
--- a/outputs/matrices.xlsx
+++ b/outputs/matrices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R-local-git\parametra\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9FC182-41A2-480D-A148-7DB0B1A2D7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F925DA16-6096-4366-86D4-F058839D8177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29835" yWindow="1860" windowWidth="29010" windowHeight="15210" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="param" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="150">
   <si>
     <t>Basic reproduction number</t>
   </si>
@@ -219,9 +219,6 @@
     <t>Questionairre</t>
   </si>
   <si>
-    <t>Experimental lab</t>
-  </si>
-  <si>
     <t>WOAH Technical Disease Card</t>
   </si>
   <si>
@@ -487,6 +484,15 @@
   </si>
   <si>
     <t>SOEI, SUD, SLICE</t>
+  </si>
+  <si>
+    <t>Systematic Review</t>
+  </si>
+  <si>
+    <t>Comparative</t>
+  </si>
+  <si>
+    <t>Manufacturer Claim</t>
   </si>
 </sst>
 </file>
@@ -566,7 +572,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -923,12 +929,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1018,36 +1037,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1081,16 +1070,49 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1384,28 +1406,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="42"/>
+      <c r="T1" s="42"/>
+      <c r="U1" s="42"/>
+      <c r="V1" s="42"/>
     </row>
     <row r="2" spans="1:23" ht="252.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
@@ -1467,8 +1489,8 @@
       <c r="V2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="W2" s="33" t="s">
-        <v>130</v>
+      <c r="W2" s="44" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1550,10 +1572,10 @@
         <f>_xlfn.XLOOKUP(V2,parameter_n_ref!$A$2:$A$20,parameter_n_ref!$C$2:$C$20)</f>
         <v>67</v>
       </c>
-      <c r="W3" s="33"/>
+      <c r="W3" s="44"/>
     </row>
     <row r="4" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="43" t="s">
         <v>40</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1622,7 +1644,7 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
@@ -1689,7 +1711,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
+      <c r="A6" s="43"/>
       <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
@@ -1756,7 +1778,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
@@ -1823,7 +1845,7 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
@@ -1890,7 +1912,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="3" t="s">
         <v>24</v>
       </c>
@@ -1957,7 +1979,7 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="3" t="s">
         <v>25</v>
       </c>
@@ -2024,7 +2046,7 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="3" t="s">
         <v>26</v>
       </c>
@@ -2091,7 +2113,7 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="3" t="s">
         <v>27</v>
       </c>
@@ -2158,7 +2180,7 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="3" t="s">
         <v>28</v>
       </c>
@@ -2225,7 +2247,7 @@
       </c>
     </row>
     <row r="14" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="3" t="s">
         <v>29</v>
       </c>
@@ -2292,7 +2314,7 @@
       </c>
     </row>
     <row r="15" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
+      <c r="A15" s="43"/>
       <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
@@ -2359,7 +2381,7 @@
       </c>
     </row>
     <row r="16" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="3" t="s">
         <v>31</v>
       </c>
@@ -2426,7 +2448,7 @@
       </c>
     </row>
     <row r="17" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="3" t="s">
         <v>32</v>
       </c>
@@ -2493,7 +2515,7 @@
       </c>
     </row>
     <row r="18" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="3" t="s">
         <v>33</v>
       </c>
@@ -2560,9 +2582,9 @@
       </c>
     </row>
     <row r="19" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="25">
         <f>_xlfn.XLOOKUP(B19,pathogen_n_ref!$A$2:$A$24,pathogen_n_ref!$C$2:$C$24)</f>
@@ -2627,7 +2649,7 @@
       </c>
     </row>
     <row r="20" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="3" t="s">
         <v>34</v>
       </c>
@@ -2694,7 +2716,7 @@
       </c>
     </row>
     <row r="21" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
+      <c r="A21" s="43"/>
       <c r="B21" s="3" t="s">
         <v>35</v>
       </c>
@@ -2761,7 +2783,7 @@
       </c>
     </row>
     <row r="22" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
+      <c r="A22" s="43"/>
       <c r="B22" s="3" t="s">
         <v>36</v>
       </c>
@@ -2828,7 +2850,7 @@
       </c>
     </row>
     <row r="23" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="3" t="s">
         <v>37</v>
       </c>
@@ -2895,7 +2917,7 @@
       </c>
     </row>
     <row r="24" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
+      <c r="A24" s="43"/>
       <c r="B24" s="3" t="s">
         <v>38</v>
       </c>
@@ -2962,12 +2984,12 @@
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="C25" s="45"/>
+      <c r="L25" s="9" t="s">
         <v>131</v>
-      </c>
-      <c r="C25" s="34"/>
-      <c r="L25" s="9" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
@@ -2998,340 +3020,366 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98162EC0-62B3-4438-BB24-FB59E4D25660}">
-  <dimension ref="A1:V20"/>
+  <dimension ref="A1:X20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="X18" sqref="X18:X21"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="22" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" customWidth="1"/>
+    <col min="5" max="23" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="172.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="172.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4">
+        <v>175</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0</v>
+      </c>
+      <c r="O2" s="4">
+        <v>0</v>
+      </c>
+      <c r="P2" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>0</v>
+      </c>
+      <c r="R2" s="4">
+        <v>0</v>
+      </c>
+      <c r="S2" s="4">
+        <v>0</v>
+      </c>
+      <c r="T2" s="4">
+        <v>0</v>
+      </c>
+      <c r="U2" s="4">
+        <v>0</v>
+      </c>
+      <c r="V2" s="4">
+        <v>0</v>
+      </c>
+      <c r="W2" s="4">
+        <v>0</v>
+      </c>
+      <c r="X2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>72</v>
+      </c>
+      <c r="C3" s="4">
+        <v>147</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>28</v>
+      </c>
+      <c r="G3" s="4">
+        <v>64</v>
+      </c>
+      <c r="H3" s="4">
+        <v>31</v>
+      </c>
+      <c r="I3" s="4">
+        <v>33</v>
+      </c>
+      <c r="J3" s="4">
+        <v>45</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4">
+        <v>19</v>
+      </c>
+      <c r="N3" s="4">
+        <v>13</v>
+      </c>
+      <c r="O3" s="4">
+        <v>2</v>
+      </c>
+      <c r="P3" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>0</v>
+      </c>
+      <c r="R3" s="4">
+        <v>0</v>
+      </c>
+      <c r="S3" s="4">
+        <v>0</v>
+      </c>
+      <c r="T3" s="4">
+        <v>0</v>
+      </c>
+      <c r="U3" s="4">
+        <v>0</v>
+      </c>
+      <c r="V3" s="4">
+        <v>0</v>
+      </c>
+      <c r="W3" s="4">
+        <v>0</v>
+      </c>
+      <c r="X3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
         <v>42</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4">
-        <v>399</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0</v>
-      </c>
-      <c r="H2" s="4">
-        <v>0</v>
-      </c>
-      <c r="I2" s="4">
-        <v>0</v>
-      </c>
-      <c r="J2" s="4">
-        <v>0</v>
-      </c>
-      <c r="K2" s="4">
-        <v>0</v>
-      </c>
-      <c r="L2" s="4">
-        <v>0</v>
-      </c>
-      <c r="M2" s="4">
-        <v>0</v>
-      </c>
-      <c r="N2" s="4">
-        <v>0</v>
-      </c>
-      <c r="O2" s="4">
-        <v>0</v>
-      </c>
-      <c r="P2" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="4">
-        <v>0</v>
-      </c>
-      <c r="R2" s="4">
-        <v>0</v>
-      </c>
-      <c r="S2" s="4">
-        <v>0</v>
-      </c>
-      <c r="T2" s="4">
-        <v>0</v>
-      </c>
-      <c r="U2" s="4">
-        <v>0</v>
-      </c>
-      <c r="V2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>111</v>
+      </c>
+      <c r="E4" s="4">
+        <v>90</v>
+      </c>
+      <c r="F4" s="4">
+        <v>84</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>41</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="4">
+        <v>0</v>
+      </c>
+      <c r="P4" s="4">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>10</v>
+      </c>
+      <c r="R4" s="4">
+        <v>8</v>
+      </c>
+      <c r="S4" s="4">
+        <v>0</v>
+      </c>
+      <c r="T4" s="4">
+        <v>0</v>
+      </c>
+      <c r="U4" s="4">
+        <v>0</v>
+      </c>
+      <c r="V4" s="4">
+        <v>0</v>
+      </c>
+      <c r="W4" s="4">
+        <v>0</v>
+      </c>
+      <c r="X4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4">
-        <v>324</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0</v>
-      </c>
-      <c r="H3" s="4">
-        <v>0</v>
-      </c>
-      <c r="I3" s="4">
-        <v>0</v>
-      </c>
-      <c r="J3" s="4">
-        <v>0</v>
-      </c>
-      <c r="K3" s="4">
-        <v>0</v>
-      </c>
-      <c r="L3" s="4">
-        <v>0</v>
-      </c>
-      <c r="M3" s="4">
-        <v>0</v>
-      </c>
-      <c r="N3" s="4">
-        <v>0</v>
-      </c>
-      <c r="O3" s="4">
-        <v>0</v>
-      </c>
-      <c r="P3" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="4">
-        <v>0</v>
-      </c>
-      <c r="R3" s="4">
-        <v>0</v>
-      </c>
-      <c r="S3" s="4">
-        <v>0</v>
-      </c>
-      <c r="T3" s="4">
-        <v>0</v>
-      </c>
-      <c r="U3" s="4">
-        <v>0</v>
-      </c>
-      <c r="V3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B5" s="4">
+        <v>33</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>101</v>
+      </c>
+      <c r="E5" s="4">
+        <v>64</v>
+      </c>
+      <c r="F5" s="4">
+        <v>79</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>30</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0</v>
+      </c>
+      <c r="O5" s="4">
+        <v>0</v>
+      </c>
+      <c r="P5" s="4">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="4">
         <v>5</v>
       </c>
-      <c r="B4" s="4">
-        <v>175</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="4">
-        <v>0</v>
-      </c>
-      <c r="J4" s="4">
-        <v>0</v>
-      </c>
-      <c r="K4" s="4">
-        <v>0</v>
-      </c>
-      <c r="L4" s="4">
-        <v>0</v>
-      </c>
-      <c r="M4" s="4">
-        <v>0</v>
-      </c>
-      <c r="N4" s="4">
-        <v>0</v>
-      </c>
-      <c r="O4" s="4">
-        <v>0</v>
-      </c>
-      <c r="P4" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="4">
-        <v>0</v>
-      </c>
-      <c r="R4" s="4">
-        <v>0</v>
-      </c>
-      <c r="S4" s="4">
-        <v>0</v>
-      </c>
-      <c r="T4" s="4">
-        <v>0</v>
-      </c>
-      <c r="U4" s="4">
-        <v>0</v>
-      </c>
-      <c r="V4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="4">
-        <v>72</v>
-      </c>
-      <c r="C5" s="4">
-        <v>149</v>
-      </c>
-      <c r="D5" s="4">
-        <v>65</v>
-      </c>
-      <c r="E5" s="4">
-        <v>31</v>
-      </c>
-      <c r="F5" s="4">
-        <v>33</v>
-      </c>
-      <c r="G5" s="4">
-        <v>28</v>
-      </c>
-      <c r="H5" s="4">
-        <v>45</v>
-      </c>
-      <c r="I5" s="4">
-        <v>0</v>
-      </c>
-      <c r="J5" s="4">
-        <v>0</v>
-      </c>
-      <c r="K5" s="4">
-        <v>13</v>
-      </c>
-      <c r="L5" s="4">
-        <v>20</v>
-      </c>
-      <c r="M5" s="4">
-        <v>2</v>
-      </c>
-      <c r="N5" s="4">
-        <v>0</v>
-      </c>
-      <c r="O5" s="4">
-        <v>0</v>
-      </c>
-      <c r="P5" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="4">
-        <v>0</v>
-      </c>
       <c r="R5" s="4">
         <v>0</v>
       </c>
@@ -3347,8 +3395,14 @@
       <c r="V5" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="W5" s="4">
+        <v>0</v>
+      </c>
+      <c r="X5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -3359,40 +3413,40 @@
         <v>91</v>
       </c>
       <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>47</v>
+      </c>
+      <c r="G6" s="4">
         <v>16</v>
       </c>
-      <c r="E6" s="4">
+      <c r="H6" s="4">
         <v>53</v>
       </c>
-      <c r="F6" s="4">
+      <c r="I6" s="4">
         <v>34</v>
       </c>
-      <c r="G6" s="4">
-        <v>47</v>
-      </c>
-      <c r="H6" s="4">
+      <c r="J6" s="4">
         <v>19</v>
       </c>
-      <c r="I6" s="4">
-        <v>0</v>
-      </c>
-      <c r="J6" s="4">
-        <v>0</v>
-      </c>
       <c r="K6" s="4">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="L6" s="4">
+        <v>0</v>
+      </c>
+      <c r="M6" s="4">
         <v>14</v>
       </c>
-      <c r="M6" s="4">
-        <v>2</v>
-      </c>
       <c r="N6" s="4">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O6" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P6" s="4">
         <v>0</v>
@@ -3415,47 +3469,53 @@
       <c r="V6" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="W6" s="4">
+        <v>0</v>
+      </c>
+      <c r="X6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="4">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="4">
         <v>28</v>
       </c>
       <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>29</v>
+      </c>
+      <c r="G7" s="4">
         <v>21</v>
       </c>
-      <c r="E7" s="4">
+      <c r="H7" s="4">
         <v>41</v>
       </c>
-      <c r="F7" s="4">
-        <v>51</v>
-      </c>
-      <c r="G7" s="4">
-        <v>29</v>
-      </c>
-      <c r="H7" s="4">
-        <v>2</v>
-      </c>
       <c r="I7" s="4">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="J7" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K7" s="4">
         <v>0</v>
       </c>
       <c r="L7" s="4">
+        <v>0</v>
+      </c>
+      <c r="M7" s="4">
         <v>10</v>
       </c>
-      <c r="M7" s="4">
-        <v>0</v>
-      </c>
       <c r="N7" s="4">
         <v>0</v>
       </c>
@@ -3483,8 +3543,14 @@
       <c r="V7" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="W7" s="4">
+        <v>0</v>
+      </c>
+      <c r="X7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -3495,22 +3561,22 @@
         <v>9</v>
       </c>
       <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>31</v>
+      </c>
+      <c r="G8" s="4">
         <v>6</v>
       </c>
-      <c r="E8" s="4">
+      <c r="H8" s="4">
         <v>22</v>
       </c>
-      <c r="F8" s="4">
-        <v>47</v>
-      </c>
-      <c r="G8" s="4">
-        <v>31</v>
-      </c>
-      <c r="H8" s="4">
-        <v>0</v>
-      </c>
       <c r="I8" s="4">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="J8" s="4">
         <v>0</v>
@@ -3519,26 +3585,26 @@
         <v>0</v>
       </c>
       <c r="L8" s="4">
+        <v>0</v>
+      </c>
+      <c r="M8" s="4">
         <v>5</v>
       </c>
-      <c r="M8" s="4">
-        <v>0</v>
-      </c>
       <c r="N8" s="4">
         <v>0</v>
       </c>
       <c r="O8" s="4">
+        <v>0</v>
+      </c>
+      <c r="P8" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>0</v>
+      </c>
+      <c r="R8" s="4">
         <v>3</v>
       </c>
-      <c r="P8" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="4">
-        <v>0</v>
-      </c>
-      <c r="R8" s="4">
-        <v>0</v>
-      </c>
       <c r="S8" s="4">
         <v>0</v>
       </c>
@@ -3551,8 +3617,14 @@
       <c r="V8" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="W8" s="4">
+        <v>0</v>
+      </c>
+      <c r="X8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -3569,7 +3641,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -3578,17 +3650,17 @@
         <v>0</v>
       </c>
       <c r="I9" s="4">
+        <v>2</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
         <v>37</v>
       </c>
-      <c r="J9" s="4">
+      <c r="L9" s="4">
         <v>31</v>
       </c>
-      <c r="K9" s="4">
-        <v>0</v>
-      </c>
-      <c r="L9" s="4">
-        <v>0</v>
-      </c>
       <c r="M9" s="4">
         <v>0</v>
       </c>
@@ -3596,31 +3668,37 @@
         <v>0</v>
       </c>
       <c r="O9" s="4">
+        <v>0</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>0</v>
+      </c>
+      <c r="R9" s="4">
         <v>3</v>
       </c>
-      <c r="P9" s="4">
-        <v>2</v>
-      </c>
-      <c r="Q9" s="4">
-        <v>0</v>
-      </c>
-      <c r="R9" s="4">
-        <v>1</v>
-      </c>
       <c r="S9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T9" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U9" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V9" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="W9" s="4">
+        <v>1</v>
+      </c>
+      <c r="X9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -3631,40 +3709,40 @@
         <v>34</v>
       </c>
       <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>4</v>
+      </c>
+      <c r="G10" s="4">
         <v>10</v>
       </c>
-      <c r="E10" s="4">
-        <v>0</v>
-      </c>
-      <c r="F10" s="4">
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
         <v>21</v>
       </c>
-      <c r="G10" s="4">
-        <v>4</v>
-      </c>
-      <c r="H10" s="4">
+      <c r="J10" s="4">
         <v>5</v>
       </c>
-      <c r="I10" s="4">
-        <v>0</v>
-      </c>
-      <c r="J10" s="4">
+      <c r="K10" s="4">
+        <v>0</v>
+      </c>
+      <c r="L10" s="4">
         <v>6</v>
       </c>
-      <c r="K10" s="4">
-        <v>0</v>
-      </c>
-      <c r="L10" s="4">
+      <c r="M10" s="4">
         <v>17</v>
       </c>
-      <c r="M10" s="4">
-        <v>6</v>
-      </c>
       <c r="N10" s="4">
         <v>0</v>
       </c>
       <c r="O10" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="P10" s="4">
         <v>0</v>
@@ -3682,13 +3760,19 @@
         <v>0</v>
       </c>
       <c r="U10" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V10" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="W10" s="4">
+        <v>0</v>
+      </c>
+      <c r="X10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -3699,22 +3783,22 @@
         <v>0</v>
       </c>
       <c r="D11" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="4">
         <v>0</v>
       </c>
       <c r="F11" s="4">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="G11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="4">
         <v>0</v>
       </c>
       <c r="I11" s="4">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="J11" s="4">
         <v>0</v>
@@ -3755,13 +3839,19 @@
       <c r="V11" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="W11" s="4">
+        <v>0</v>
+      </c>
+      <c r="X11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="4">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="4">
         <v>0</v>
@@ -3773,17 +3863,17 @@
         <v>0</v>
       </c>
       <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
         <v>4</v>
       </c>
-      <c r="G12" s="4">
-        <v>0</v>
-      </c>
-      <c r="H12" s="4">
-        <v>0</v>
-      </c>
-      <c r="I12" s="4">
-        <v>0</v>
-      </c>
       <c r="J12" s="4">
         <v>0</v>
       </c>
@@ -3823,8 +3913,14 @@
       <c r="V12" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="W12" s="4">
+        <v>0</v>
+      </c>
+      <c r="X12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
@@ -3835,23 +3931,23 @@
         <v>15</v>
       </c>
       <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
         <v>28</v>
       </c>
-      <c r="E13" s="4">
-        <v>0</v>
-      </c>
-      <c r="F13" s="4">
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
         <v>15</v>
       </c>
-      <c r="G13" s="4">
-        <v>0</v>
-      </c>
-      <c r="H13" s="4">
-        <v>0</v>
-      </c>
-      <c r="I13" s="4">
-        <v>0</v>
-      </c>
       <c r="J13" s="4">
         <v>0</v>
       </c>
@@ -3859,11 +3955,11 @@
         <v>0</v>
       </c>
       <c r="L13" s="4">
+        <v>0</v>
+      </c>
+      <c r="M13" s="4">
         <v>12</v>
       </c>
-      <c r="M13" s="4">
-        <v>0</v>
-      </c>
       <c r="N13" s="4">
         <v>0</v>
       </c>
@@ -3891,8 +3987,14 @@
       <c r="V13" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="W13" s="4">
+        <v>0</v>
+      </c>
+      <c r="X13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -3903,7 +4005,7 @@
         <v>4</v>
       </c>
       <c r="D14" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="4">
         <v>0</v>
@@ -3912,7 +4014,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="4">
         <v>0</v>
@@ -3927,20 +4029,20 @@
         <v>0</v>
       </c>
       <c r="L14" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="4">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="N14" s="4">
+        <v>0</v>
+      </c>
+      <c r="O14" s="4">
+        <v>18</v>
+      </c>
+      <c r="P14" s="4">
         <v>16</v>
       </c>
-      <c r="O14" s="4">
-        <v>0</v>
-      </c>
-      <c r="P14" s="4">
-        <v>0</v>
-      </c>
       <c r="Q14" s="4">
         <v>0</v>
       </c>
@@ -3957,10 +4059,16 @@
         <v>0</v>
       </c>
       <c r="V14" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="W14" s="4">
+        <v>0</v>
+      </c>
+      <c r="X14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
@@ -3971,28 +4079,28 @@
         <v>16</v>
       </c>
       <c r="D15" s="4">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
         <v>3</v>
       </c>
-      <c r="E15" s="4">
-        <v>0</v>
-      </c>
-      <c r="F15" s="4">
-        <v>0</v>
-      </c>
-      <c r="G15" s="4">
-        <v>0</v>
-      </c>
       <c r="H15" s="4">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I15" s="4">
         <v>0</v>
       </c>
       <c r="J15" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K15" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" s="4">
         <v>0</v>
@@ -4001,7 +4109,7 @@
         <v>0</v>
       </c>
       <c r="N15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15" s="4">
         <v>0</v>
@@ -4027,8 +4135,14 @@
       <c r="V15" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="W15" s="4">
+        <v>0</v>
+      </c>
+      <c r="X15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -4039,17 +4153,17 @@
         <v>15</v>
       </c>
       <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
         <v>3</v>
       </c>
-      <c r="E16" s="4">
-        <v>0</v>
-      </c>
-      <c r="F16" s="4">
-        <v>0</v>
-      </c>
-      <c r="G16" s="4">
-        <v>0</v>
-      </c>
       <c r="H16" s="4">
         <v>0</v>
       </c>
@@ -4095,8 +4209,14 @@
       <c r="V16" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="W16" s="4">
+        <v>0</v>
+      </c>
+      <c r="X16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -4134,14 +4254,14 @@
         <v>0</v>
       </c>
       <c r="M17" s="4">
+        <v>0</v>
+      </c>
+      <c r="N17" s="4">
+        <v>0</v>
+      </c>
+      <c r="O17" s="4">
         <v>3</v>
       </c>
-      <c r="N17" s="4">
-        <v>0</v>
-      </c>
-      <c r="O17" s="4">
-        <v>0</v>
-      </c>
       <c r="P17" s="4">
         <v>0</v>
       </c>
@@ -4163,8 +4283,14 @@
       <c r="V17" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="W17" s="4">
+        <v>0</v>
+      </c>
+      <c r="X17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
@@ -4175,17 +4301,17 @@
         <v>0</v>
       </c>
       <c r="D18" s="4">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
         <v>3</v>
       </c>
-      <c r="E18" s="4">
-        <v>0</v>
-      </c>
-      <c r="F18" s="4">
-        <v>0</v>
-      </c>
-      <c r="G18" s="4">
-        <v>0</v>
-      </c>
       <c r="H18" s="4">
         <v>0</v>
       </c>
@@ -4199,10 +4325,10 @@
         <v>0</v>
       </c>
       <c r="L18" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N18" s="4">
         <v>0</v>
@@ -4231,8 +4357,14 @@
       <c r="V18" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="W18" s="4">
+        <v>0</v>
+      </c>
+      <c r="X18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -4282,7 +4414,7 @@
         <v>0</v>
       </c>
       <c r="Q19" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R19" s="4">
         <v>0</v>
@@ -4291,7 +4423,7 @@
         <v>0</v>
       </c>
       <c r="T19" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U19" s="4">
         <v>0</v>
@@ -4299,8 +4431,14 @@
       <c r="V19" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="W19" s="4">
+        <v>0</v>
+      </c>
+      <c r="X19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
@@ -4323,22 +4461,22 @@
         <v>0</v>
       </c>
       <c r="H20" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" s="4">
         <v>0</v>
       </c>
       <c r="J20" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="4">
         <v>0</v>
       </c>
       <c r="L20" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M20" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N20" s="4">
         <v>0</v>
@@ -4367,9 +4505,15 @@
       <c r="V20" s="4">
         <v>0</v>
       </c>
+      <c r="W20" s="4">
+        <v>0</v>
+      </c>
+      <c r="X20" s="4">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:V20">
+  <conditionalFormatting sqref="C2:X20">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -4389,19 +4533,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D22E2B9B-73A2-43E9-BAF1-CF037AA0748E}">
   <dimension ref="B2:V24"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="Z5" sqref="Z5"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="22" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:22" ht="162" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>42</v>
@@ -4455,146 +4599,147 @@
         <v>53</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="49"/>
-      <c r="D3" s="35" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="38" t="s">
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="J3" s="38"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="40" t="s">
+      <c r="J3" s="49"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="40" t="s">
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="50"/>
+      <c r="R3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="38"/>
-      <c r="T3" s="38"/>
-      <c r="U3" s="38"/>
-      <c r="V3" s="39"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="50"/>
     </row>
     <row r="4" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="47">
-        <v>224</v>
-      </c>
-      <c r="D4" s="41">
-        <v>134</v>
-      </c>
-      <c r="E4" s="42">
-        <v>0</v>
-      </c>
-      <c r="F4" s="42">
-        <v>42</v>
-      </c>
-      <c r="G4" s="42">
-        <v>0</v>
-      </c>
-      <c r="H4" s="43">
-        <v>0</v>
-      </c>
-      <c r="I4" s="42">
-        <v>0</v>
-      </c>
-      <c r="J4" s="42">
-        <v>1</v>
-      </c>
-      <c r="K4" s="43">
-        <v>0</v>
-      </c>
-      <c r="L4" s="44">
-        <v>147</v>
-      </c>
-      <c r="M4" s="42">
-        <v>13</v>
-      </c>
-      <c r="N4" s="42">
-        <v>0</v>
-      </c>
-      <c r="O4" s="42">
-        <v>0</v>
-      </c>
-      <c r="P4" s="42">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="43">
-        <v>0</v>
-      </c>
-      <c r="R4" s="41">
-        <v>0</v>
-      </c>
-      <c r="S4" s="42">
-        <v>0</v>
-      </c>
-      <c r="T4" s="42">
-        <v>0</v>
-      </c>
-      <c r="U4" s="42">
-        <v>0</v>
-      </c>
-      <c r="V4" s="43">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="C4" s="54">
+        <v>6</v>
+      </c>
+      <c r="D4" s="31">
+        <v>0</v>
+      </c>
+      <c r="E4" s="32">
+        <v>0</v>
+      </c>
+      <c r="F4" s="32">
+        <v>0</v>
+      </c>
+      <c r="G4" s="32">
+        <v>11</v>
+      </c>
+      <c r="H4" s="33">
+        <v>1</v>
+      </c>
+      <c r="I4" s="32">
+        <v>2</v>
+      </c>
+      <c r="J4" s="32">
+        <v>3</v>
+      </c>
+      <c r="K4" s="33">
+        <v>0</v>
+      </c>
+      <c r="L4" s="34">
+        <v>0</v>
+      </c>
+      <c r="M4" s="32">
+        <v>70</v>
+      </c>
+      <c r="N4" s="32">
+        <v>3</v>
+      </c>
+      <c r="O4" s="32">
+        <v>0</v>
+      </c>
+      <c r="P4" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="33">
+        <v>0</v>
+      </c>
+      <c r="R4" s="31">
+        <v>4</v>
+      </c>
+      <c r="S4" s="32">
+        <v>0</v>
+      </c>
+      <c r="T4" s="32">
+        <v>0</v>
+      </c>
+      <c r="U4" s="32">
+        <v>0</v>
+      </c>
+      <c r="V4" s="33">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="47">
-        <v>221</v>
+        <v>19</v>
+      </c>
+      <c r="C5" s="37">
+        <v>192</v>
       </c>
       <c r="D5" s="26">
-        <v>0</v>
+        <v>134</v>
       </c>
       <c r="E5" s="6">
         <v>0</v>
       </c>
       <c r="F5" s="6">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="G5" s="6">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="H5" s="27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J5" s="6">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="K5" s="27">
         <v>0</v>
       </c>
-      <c r="L5" s="45">
-        <v>0</v>
+      <c r="L5" s="35">
+        <v>147</v>
       </c>
       <c r="M5" s="6">
-        <v>72</v>
+        <v>13</v>
       </c>
       <c r="N5" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O5" s="6">
         <v>0</v>
@@ -4606,7 +4751,7 @@
         <v>0</v>
       </c>
       <c r="R5" s="26">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="S5" s="6">
         <v>0</v>
@@ -4618,27 +4763,27 @@
         <v>0</v>
       </c>
       <c r="V5" s="27">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="47">
-        <v>209</v>
+      <c r="C6" s="37">
+        <v>2</v>
       </c>
       <c r="D6" s="26">
-        <v>0</v>
+        <v>142</v>
       </c>
       <c r="E6" s="6">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F6" s="6">
         <v>0</v>
       </c>
       <c r="G6" s="6">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H6" s="27">
         <v>1</v>
@@ -4650,9 +4795,9 @@
         <v>0</v>
       </c>
       <c r="K6" s="27">
-        <v>3</v>
-      </c>
-      <c r="L6" s="45">
+        <v>11</v>
+      </c>
+      <c r="L6" s="35">
         <v>0</v>
       </c>
       <c r="M6" s="6">
@@ -4683,18 +4828,18 @@
         <v>0</v>
       </c>
       <c r="V6" s="27">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="47">
-        <v>121</v>
+      <c r="C7" s="37">
+        <v>17</v>
       </c>
       <c r="D7" s="26">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E7" s="6">
         <v>0</v>
@@ -4709,7 +4854,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="6">
-        <v>35</v>
+        <v>106</v>
       </c>
       <c r="J7" s="6">
         <v>1</v>
@@ -4717,7 +4862,7 @@
       <c r="K7" s="27">
         <v>1</v>
       </c>
-      <c r="L7" s="45">
+      <c r="L7" s="35">
         <v>0</v>
       </c>
       <c r="M7" s="6">
@@ -4755,8 +4900,8 @@
       <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="47">
-        <v>101</v>
+      <c r="C8" s="37">
+        <v>97</v>
       </c>
       <c r="D8" s="26">
         <v>0</v>
@@ -4774,7 +4919,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="6">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J8" s="6">
         <v>1</v>
@@ -4782,7 +4927,7 @@
       <c r="K8" s="27">
         <v>0</v>
       </c>
-      <c r="L8" s="45">
+      <c r="L8" s="35">
         <v>0</v>
       </c>
       <c r="M8" s="6">
@@ -4820,11 +4965,11 @@
       <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="47">
-        <v>60</v>
+      <c r="C9" s="37">
+        <v>37</v>
       </c>
       <c r="D9" s="26">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E9" s="6">
         <v>3</v>
@@ -4839,7 +4984,7 @@
         <v>3</v>
       </c>
       <c r="I9" s="6">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="J9" s="6">
         <v>3</v>
@@ -4847,7 +4992,7 @@
       <c r="K9" s="27">
         <v>0</v>
       </c>
-      <c r="L9" s="45">
+      <c r="L9" s="35">
         <v>0</v>
       </c>
       <c r="M9" s="6">
@@ -4883,16 +5028,16 @@
     </row>
     <row r="10" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="47">
-        <v>49</v>
+        <v>28</v>
+      </c>
+      <c r="C10" s="37">
+        <v>1</v>
       </c>
       <c r="D10" s="26">
         <v>0</v>
       </c>
       <c r="E10" s="6">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="F10" s="6">
         <v>0</v>
@@ -4901,25 +5046,25 @@
         <v>0</v>
       </c>
       <c r="H10" s="27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I10" s="6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J10" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K10" s="27">
         <v>0</v>
       </c>
-      <c r="L10" s="45">
+      <c r="L10" s="35">
         <v>0</v>
       </c>
       <c r="M10" s="6">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="N10" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O10" s="6">
         <v>0</v>
@@ -4931,7 +5076,7 @@
         <v>0</v>
       </c>
       <c r="R10" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S10" s="6">
         <v>0</v>
@@ -4948,43 +5093,43 @@
     </row>
     <row r="11" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="47">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="C11" s="37">
+        <v>39</v>
       </c>
       <c r="D11" s="26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E11" s="6">
+        <v>0</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0</v>
+      </c>
+      <c r="H11" s="27">
+        <v>3</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0</v>
+      </c>
+      <c r="K11" s="27">
+        <v>0</v>
+      </c>
+      <c r="L11" s="35">
+        <v>0</v>
+      </c>
+      <c r="M11" s="6">
         <v>47</v>
       </c>
-      <c r="F11" s="6">
-        <v>0</v>
-      </c>
-      <c r="G11" s="6">
-        <v>0</v>
-      </c>
-      <c r="H11" s="27">
-        <v>2</v>
-      </c>
-      <c r="I11" s="6">
-        <v>5</v>
-      </c>
-      <c r="J11" s="6">
-        <v>2</v>
-      </c>
-      <c r="K11" s="27">
-        <v>0</v>
-      </c>
-      <c r="L11" s="45">
-        <v>0</v>
-      </c>
-      <c r="M11" s="6">
-        <v>0</v>
-      </c>
       <c r="N11" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O11" s="6">
         <v>0</v>
@@ -4996,7 +5141,7 @@
         <v>0</v>
       </c>
       <c r="R11" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S11" s="6">
         <v>0</v>
@@ -5013,28 +5158,28 @@
     </row>
     <row r="12" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="47">
-        <v>44</v>
+        <v>27</v>
+      </c>
+      <c r="C12" s="37">
+        <v>15</v>
       </c>
       <c r="D12" s="26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12" s="6">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F12" s="6">
         <v>0</v>
       </c>
       <c r="G12" s="6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H12" s="27">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I12" s="6">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="J12" s="6">
         <v>1</v>
@@ -5042,14 +5187,14 @@
       <c r="K12" s="27">
         <v>0</v>
       </c>
-      <c r="L12" s="45">
+      <c r="L12" s="35">
         <v>0</v>
       </c>
       <c r="M12" s="6">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N12" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O12" s="6">
         <v>0</v>
@@ -5061,7 +5206,7 @@
         <v>0</v>
       </c>
       <c r="R12" s="26">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="S12" s="6">
         <v>0</v>
@@ -5073,48 +5218,48 @@
         <v>0</v>
       </c>
       <c r="V12" s="27">
-        <v>0</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="47">
-        <v>75</v>
+        <v>24</v>
+      </c>
+      <c r="C13" s="37">
+        <v>10</v>
       </c>
       <c r="D13" s="26">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E13" s="6">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="F13" s="6">
         <v>0</v>
       </c>
       <c r="G13" s="6">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="H13" s="27">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I13" s="6">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="J13" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" s="27">
-        <v>0</v>
-      </c>
-      <c r="L13" s="45">
+        <v>1</v>
+      </c>
+      <c r="L13" s="35">
         <v>0</v>
       </c>
       <c r="M13" s="6">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="N13" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O13" s="6">
         <v>0</v>
@@ -5126,7 +5271,7 @@
         <v>0</v>
       </c>
       <c r="R13" s="26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S13" s="6">
         <v>0</v>
@@ -5138,45 +5283,45 @@
         <v>0</v>
       </c>
       <c r="V13" s="27">
-        <v>43</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="47">
-        <v>19</v>
+        <v>29</v>
+      </c>
+      <c r="C14" s="37">
+        <v>37</v>
       </c>
       <c r="D14" s="26">
         <v>0</v>
       </c>
       <c r="E14" s="6">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="F14" s="6">
         <v>0</v>
       </c>
       <c r="G14" s="6">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="H14" s="27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I14" s="6">
         <v>1</v>
       </c>
       <c r="J14" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="27">
-        <v>1</v>
-      </c>
-      <c r="L14" s="45">
+        <v>0</v>
+      </c>
+      <c r="L14" s="35">
         <v>0</v>
       </c>
       <c r="M14" s="6">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="N14" s="6">
         <v>0</v>
@@ -5191,7 +5336,7 @@
         <v>0</v>
       </c>
       <c r="R14" s="26">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="S14" s="6">
         <v>0</v>
@@ -5208,16 +5353,16 @@
     </row>
     <row r="15" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="47">
-        <v>26</v>
+        <v>34</v>
+      </c>
+      <c r="C15" s="37">
+        <v>23</v>
       </c>
       <c r="D15" s="26">
         <v>0</v>
       </c>
       <c r="E15" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="6">
         <v>0</v>
@@ -5226,25 +5371,25 @@
         <v>0</v>
       </c>
       <c r="H15" s="27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I15" s="6">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J15" s="6">
         <v>0</v>
       </c>
       <c r="K15" s="27">
-        <v>0</v>
-      </c>
-      <c r="L15" s="45">
+        <v>1</v>
+      </c>
+      <c r="L15" s="35">
         <v>0</v>
       </c>
       <c r="M15" s="6">
         <v>0</v>
       </c>
       <c r="N15" s="6">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O15" s="6">
         <v>0</v>
@@ -5259,7 +5404,7 @@
         <v>0</v>
       </c>
       <c r="S15" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T15" s="6">
         <v>0</v>
@@ -5268,21 +5413,21 @@
         <v>0</v>
       </c>
       <c r="V15" s="27">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="47">
         <v>30</v>
       </c>
+      <c r="C16" s="37">
+        <v>20</v>
+      </c>
       <c r="D16" s="26">
         <v>0</v>
       </c>
       <c r="E16" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="6">
         <v>0</v>
@@ -5291,25 +5436,25 @@
         <v>0</v>
       </c>
       <c r="H16" s="27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I16" s="6">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J16" s="6">
         <v>0</v>
       </c>
       <c r="K16" s="27">
-        <v>1</v>
-      </c>
-      <c r="L16" s="45">
+        <v>0</v>
+      </c>
+      <c r="L16" s="35">
         <v>0</v>
       </c>
       <c r="M16" s="6">
         <v>0</v>
       </c>
       <c r="N16" s="6">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O16" s="6">
         <v>0</v>
@@ -5324,7 +5469,7 @@
         <v>0</v>
       </c>
       <c r="S16" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T16" s="6">
         <v>0</v>
@@ -5333,14 +5478,14 @@
         <v>0</v>
       </c>
       <c r="V16" s="27">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="47">
+      <c r="C17" s="37">
         <v>20</v>
       </c>
       <c r="D17" s="26">
@@ -5367,7 +5512,7 @@
       <c r="K17" s="27">
         <v>0</v>
       </c>
-      <c r="L17" s="45">
+      <c r="L17" s="35">
         <v>0</v>
       </c>
       <c r="M17" s="6">
@@ -5405,11 +5550,11 @@
       <c r="B18" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="47">
-        <v>7</v>
+      <c r="C18" s="37">
+        <v>2</v>
       </c>
       <c r="D18" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="6">
         <v>3</v>
@@ -5432,7 +5577,7 @@
       <c r="K18" s="27">
         <v>0</v>
       </c>
-      <c r="L18" s="45">
+      <c r="L18" s="35">
         <v>0</v>
       </c>
       <c r="M18" s="6">
@@ -5470,7 +5615,7 @@
       <c r="B19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="47">
+      <c r="C19" s="37">
         <v>6</v>
       </c>
       <c r="D19" s="26">
@@ -5497,7 +5642,7 @@
       <c r="K19" s="27">
         <v>0</v>
       </c>
-      <c r="L19" s="45">
+      <c r="L19" s="35">
         <v>0</v>
       </c>
       <c r="M19" s="6">
@@ -5533,43 +5678,43 @@
     </row>
     <row r="20" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="47">
-        <v>21</v>
+        <v>37</v>
+      </c>
+      <c r="C20" s="37">
+        <v>11</v>
       </c>
       <c r="D20" s="26">
         <v>0</v>
       </c>
       <c r="E20" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="6">
         <v>0</v>
       </c>
       <c r="G20" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J20" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K20" s="27">
         <v>0</v>
       </c>
-      <c r="L20" s="45">
+      <c r="L20" s="35">
         <v>0</v>
       </c>
       <c r="M20" s="6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N20" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O20" s="6">
         <v>0</v>
@@ -5584,57 +5729,57 @@
         <v>0</v>
       </c>
       <c r="S20" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T20" s="6">
         <v>0</v>
       </c>
       <c r="U20" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V20" s="27">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="47">
-        <v>13</v>
+        <v>59</v>
+      </c>
+      <c r="C21" s="37">
+        <v>6</v>
       </c>
       <c r="D21" s="26">
         <v>0</v>
       </c>
       <c r="E21" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" s="6">
         <v>0</v>
       </c>
       <c r="G21" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" s="27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J21" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K21" s="27">
         <v>0</v>
       </c>
-      <c r="L21" s="45">
+      <c r="L21" s="35">
         <v>0</v>
       </c>
       <c r="M21" s="6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N21" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O21" s="6">
         <v>0</v>
@@ -5649,23 +5794,23 @@
         <v>0</v>
       </c>
       <c r="S21" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T21" s="6">
         <v>0</v>
       </c>
       <c r="U21" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V21" s="27">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="47">
+      <c r="C22" s="37">
         <v>2</v>
       </c>
       <c r="D22" s="26">
@@ -5692,7 +5837,7 @@
       <c r="K22" s="27">
         <v>0</v>
       </c>
-      <c r="L22" s="45">
+      <c r="L22" s="35">
         <v>0</v>
       </c>
       <c r="M22" s="6">
@@ -5730,7 +5875,7 @@
       <c r="B23" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="47">
+      <c r="C23" s="37">
         <v>0</v>
       </c>
       <c r="D23" s="26">
@@ -5757,7 +5902,7 @@
       <c r="K23" s="27">
         <v>0</v>
       </c>
-      <c r="L23" s="45">
+      <c r="L23" s="35">
         <v>0</v>
       </c>
       <c r="M23" s="6">
@@ -5795,7 +5940,7 @@
       <c r="B24" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="48">
+      <c r="C24" s="38">
         <v>0</v>
       </c>
       <c r="D24" s="28">
@@ -5822,7 +5967,7 @@
       <c r="K24" s="30">
         <v>0</v>
       </c>
-      <c r="L24" s="46">
+      <c r="L24" s="36">
         <v>0</v>
       </c>
       <c r="M24" s="29">
@@ -5895,7 +6040,7 @@
   <sheetData>
     <row r="2" spans="2:31" ht="74.25" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D2" s="2">
         <v>1993</v>
@@ -7548,7 +7693,7 @@
     </row>
     <row r="20" spans="2:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C20" s="6">
         <v>2</v>
@@ -7957,113 +8102,113 @@
   <sheetData>
     <row r="2" spans="2:27" ht="110.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="W2" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="S2" s="2" t="s">
+      <c r="X2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="AA2" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="T2" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="Z2" s="2" t="s">
+    </row>
+    <row r="3" spans="2:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="AA2" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="2:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="35" t="s">
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="52" t="s">
+        <v>145</v>
+      </c>
+      <c r="N3" s="53"/>
+      <c r="O3" s="51" t="s">
         <v>144</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="52" t="s">
-        <v>146</v>
-      </c>
-      <c r="N3" s="53"/>
-      <c r="O3" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="40"/>
-      <c r="R3" s="38"/>
-      <c r="S3" s="38"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="35"/>
-      <c r="V3" s="37"/>
-      <c r="W3" s="35"/>
-      <c r="X3" s="36"/>
-      <c r="Y3" s="36"/>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="50"/>
+      <c r="P3" s="50"/>
+      <c r="Q3" s="51"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="50"/>
+      <c r="U3" s="46"/>
+      <c r="V3" s="48"/>
+      <c r="W3" s="46"/>
+      <c r="X3" s="47"/>
+      <c r="Y3" s="47"/>
+      <c r="Z3" s="48"/>
+      <c r="AA3" s="40"/>
     </row>
     <row r="4" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
@@ -8141,7 +8286,7 @@
       <c r="Z4" s="27">
         <v>0</v>
       </c>
-      <c r="AA4" s="51">
+      <c r="AA4" s="41">
         <v>0</v>
       </c>
     </row>
@@ -8221,7 +8366,7 @@
       <c r="Z5" s="27">
         <v>0</v>
       </c>
-      <c r="AA5" s="51">
+      <c r="AA5" s="41">
         <v>0</v>
       </c>
     </row>
@@ -8301,7 +8446,7 @@
       <c r="Z6" s="27">
         <v>1</v>
       </c>
-      <c r="AA6" s="51">
+      <c r="AA6" s="41">
         <v>0</v>
       </c>
     </row>
@@ -8381,7 +8526,7 @@
       <c r="Z7" s="27">
         <v>0</v>
       </c>
-      <c r="AA7" s="51">
+      <c r="AA7" s="41">
         <v>0</v>
       </c>
     </row>
@@ -8461,7 +8606,7 @@
       <c r="Z8" s="27">
         <v>0</v>
       </c>
-      <c r="AA8" s="51">
+      <c r="AA8" s="41">
         <v>0</v>
       </c>
     </row>
@@ -8541,7 +8686,7 @@
       <c r="Z9" s="27">
         <v>0</v>
       </c>
-      <c r="AA9" s="51">
+      <c r="AA9" s="41">
         <v>0</v>
       </c>
     </row>
@@ -8621,7 +8766,7 @@
       <c r="Z10" s="27">
         <v>0</v>
       </c>
-      <c r="AA10" s="51">
+      <c r="AA10" s="41">
         <v>0</v>
       </c>
     </row>
@@ -8701,7 +8846,7 @@
       <c r="Z11" s="27">
         <v>0</v>
       </c>
-      <c r="AA11" s="51">
+      <c r="AA11" s="41">
         <v>0</v>
       </c>
     </row>
@@ -8781,7 +8926,7 @@
       <c r="Z12" s="27">
         <v>0</v>
       </c>
-      <c r="AA12" s="51">
+      <c r="AA12" s="41">
         <v>0</v>
       </c>
     </row>
@@ -8861,13 +9006,13 @@
       <c r="Z13" s="27">
         <v>0</v>
       </c>
-      <c r="AA13" s="51">
+      <c r="AA13" s="41">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="26">
         <v>0</v>
@@ -8941,7 +9086,7 @@
       <c r="Z14" s="27">
         <v>0</v>
       </c>
-      <c r="AA14" s="51">
+      <c r="AA14" s="41">
         <v>0</v>
       </c>
     </row>
@@ -9021,7 +9166,7 @@
       <c r="Z15" s="27">
         <v>0</v>
       </c>
-      <c r="AA15" s="51">
+      <c r="AA15" s="41">
         <v>1</v>
       </c>
     </row>
@@ -9101,7 +9246,7 @@
       <c r="Z16" s="30">
         <v>0</v>
       </c>
-      <c r="AA16" s="48">
+      <c r="AA16" s="38">
         <v>0</v>
       </c>
     </row>
@@ -9114,8 +9259,8 @@
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="O3:P3"/>
   </mergeCells>
-  <conditionalFormatting sqref="L4:L16">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="C4:AA16">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9126,8 +9271,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:AA16">
-    <cfRule type="colorScale" priority="9">
+  <conditionalFormatting sqref="L4:L16">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9154,13 +9299,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" t="s">
         <v>128</v>
-      </c>
-      <c r="C1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -9389,13 +9534,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" t="s">
         <v>128</v>
-      </c>
-      <c r="C1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -9565,7 +9710,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17">
         <v>28</v>
@@ -9620,7 +9765,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -9631,7 +9776,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -9663,7 +9808,7 @@
   </sheetPr>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -9677,288 +9822,288 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="C1" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="D1" s="24" t="s">
         <v>82</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>85</v>
-      </c>
       <c r="D2" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>88</v>
-      </c>
       <c r="D4" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>91</v>
-      </c>
       <c r="D6" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>93</v>
-      </c>
       <c r="D7" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>95</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>98</v>
-      </c>
       <c r="D10" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="D11" s="13" t="s">
         <v>100</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="C12" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>104</v>
-      </c>
       <c r="D12" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B13" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="D13" s="13" t="s">
         <v>106</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="C14" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>110</v>
-      </c>
       <c r="D14" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="C15" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="C15" s="18" t="s">
-        <v>113</v>
-      </c>
       <c r="D15" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="D16" s="13" t="s">
         <v>115</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B19" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="C19" s="15" t="s">
-        <v>121</v>
-      </c>
       <c r="D19" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B20" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>123</v>
-      </c>
       <c r="D20" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>